<commit_message>
Major Rewrite of the Wasm Integer classes.
</commit_message>
<xml_diff>
--- a/spec/Wasm Variable Types.xlsx
+++ b/spec/Wasm Variable Types.xlsx
@@ -7,16 +7,112 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Wasm" sheetId="1" r:id="rId1"/>
+    <sheet name="Java" sheetId="2" r:id="rId2"/>
+    <sheet name="Sources " sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+http://webassembly.org/docs/binary-encoding/
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Note: Excel does not work with numbers larger than  2^60 or so.  Thus 2^63 and 2^24 are stored as strings.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="E7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Note: Excel does not work with numbers larger than  2^60 or so.  Thus 2^63 and 2^24 are stored as strings.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="50">
   <si>
     <t>Min Value</t>
   </si>
@@ -127,13 +223,55 @@
   </si>
   <si>
     <t>"+9,223,372,036,854,775,807"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Java Integer and Long types are signed.  </t>
+  </si>
+  <si>
+    <t>Value()</t>
+  </si>
+  <si>
+    <t>Concrete Types</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Min/MaxValue()</t>
+  </si>
+  <si>
+    <t>Constructor(Byte[])</t>
+  </si>
+  <si>
+    <t>http://webassembly.org/docs/binary-encoding/</t>
+  </si>
+  <si>
+    <t>https://webassembly.github.io/spec/binary/values.html#binary-int</t>
+  </si>
+  <si>
+    <t>https://webassembly.github.io/spec/syntax/values.html#syntax-int</t>
+  </si>
+  <si>
+    <t>hex</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>8000_0000</t>
+  </si>
+  <si>
+    <t>7FFF_FFFF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="00000"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +291,33 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -217,7 +382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -228,10 +393,34 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -535,50 +724,735 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="12">
+        <f>-2^(C2-1)</f>
+        <v>-128</v>
+      </c>
+      <c r="G2" s="12">
+        <f>2 ^(C2-1) -1</f>
+        <v>127</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>32</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12">
+        <f>-2^(C3-1)</f>
+        <v>-2147483648</v>
+      </c>
+      <c r="G3" s="12">
+        <f>2 ^(C3-1) -1</f>
+        <v>2147483647</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>63</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>64</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f>CEILING(C6/7,1)</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="12">
+        <f>-1 * (2^(C6-1))</f>
+        <v>-64</v>
+      </c>
+      <c r="G6" s="12">
+        <f>2 ^(C6-1) -1</f>
+        <v>63</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>32</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f>CEILING(C7/7,1)</f>
+        <v>5</v>
+      </c>
+      <c r="F7" s="12">
+        <f>-1 * (2^(C7-1))</f>
+        <v>-2147483648</v>
+      </c>
+      <c r="G7" s="12">
+        <f>2 ^(C7-1) -1</f>
+        <v>2147483647</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>64</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f>CEILING(C8/7,1)</f>
+        <v>10</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f>C9/8</f>
+        <v>1</v>
+      </c>
+      <c r="F9" s="12">
+        <v>0</v>
+      </c>
+      <c r="G9" s="12">
+        <f>2 ^C9 -1</f>
+        <v>255</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <f>C10/8</f>
+        <v>2</v>
+      </c>
+      <c r="F10" s="12">
+        <v>0</v>
+      </c>
+      <c r="G10" s="12">
+        <f>2 ^C10 -1</f>
+        <v>65535</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>32</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <f>C11/8</f>
+        <v>4</v>
+      </c>
+      <c r="F11" s="12">
+        <v>0</v>
+      </c>
+      <c r="G11" s="12">
+        <f>2 ^C11 -1</f>
+        <v>4294967295</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>64</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <f>C12/8</f>
+        <v>8</v>
+      </c>
+      <c r="F12" s="12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <f>CEILING(C13/7,1)</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="12">
+        <v>0</v>
+      </c>
+      <c r="G13" s="12">
+        <f>(2^C13)-1</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <f>CEILING(C14/7,1)</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="12">
+        <v>0</v>
+      </c>
+      <c r="G14" s="12">
+        <f>(2^C14)-1</f>
+        <v>127</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>32</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <f>CEILING(C15/7,1)</f>
+        <v>5</v>
+      </c>
+      <c r="F15" s="12">
+        <v>0</v>
+      </c>
+      <c r="G15" s="12">
+        <f>(2^C15)-1</f>
+        <v>4294967295</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4" s="17">
+        <v>32</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="4">
+        <f>-2^(B4-1)</f>
+        <v>-128</v>
+      </c>
+      <c r="C7" s="4">
+        <f>-2^(C4-1)</f>
+        <v>-32768</v>
+      </c>
+      <c r="D7" s="4">
+        <f>-2^(D4-1)</f>
+        <v>-2147483648</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4">
+        <f>2 ^(B4-1) -1</f>
+        <v>127</v>
+      </c>
+      <c r="C8" s="4">
+        <f>2 ^(C4-1) -1</f>
+        <v>32767</v>
+      </c>
+      <c r="D8" s="4">
+        <f>2 ^(D4-1) -1</f>
+        <v>2147483647</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="9" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
@@ -752,15 +1626,15 @@
         <v>1</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K5" si="0">K3/8</f>
+        <f>K3/8</f>
         <v>2</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:M5" si="1">L3/8</f>
+        <f>L3/8</f>
         <v>4</v>
       </c>
       <c r="M5">
-        <f t="shared" si="1"/>
+        <f>M3/8</f>
         <v>8</v>
       </c>
       <c r="N5">
@@ -768,15 +1642,15 @@
         <v>1</v>
       </c>
       <c r="O5">
-        <f t="shared" ref="O5:P5" si="2">CEILING(O3/7,1)</f>
+        <f>CEILING(O3/7,1)</f>
         <v>1</v>
       </c>
       <c r="P5">
-        <f t="shared" si="2"/>
+        <f>CEILING(P3/7,1)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
@@ -784,6 +1658,7 @@
         <f>-2^(B3-1)</f>
         <v>-128</v>
       </c>
+      <c r="C7" s="4"/>
       <c r="D7" s="4">
         <f>-2^(D3-1)</f>
         <v>-2147483648</v>
@@ -799,7 +1674,7 @@
         <v>-64</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" ref="H7" si="3">-1 * (2^(H3-1))</f>
+        <f>-1 * (2^(H3-1))</f>
         <v>-2147483648</v>
       </c>
       <c r="I7" s="4" t="s">
@@ -827,7 +1702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
@@ -835,6 +1710,7 @@
         <f>2 ^(B3-1) -1</f>
         <v>127</v>
       </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="4">
         <f>2 ^(D3-1) -1</f>
         <v>2147483647</v>
@@ -850,7 +1726,7 @@
         <v>63</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" ref="H8" si="4">2 ^(H3-1) -1</f>
+        <f>2 ^(H3-1) -1</f>
         <v>2147483647</v>
       </c>
       <c r="I8" s="4" t="s">
@@ -876,11 +1752,11 @@
         <v>1</v>
       </c>
       <c r="O8" s="4">
-        <f t="shared" ref="O8:P8" si="5">(2^O3)-1</f>
+        <f>(2^O3)-1</f>
         <v>127</v>
       </c>
       <c r="P8" s="4">
-        <f t="shared" si="5"/>
+        <f>(2^P3)-1</f>
         <v>4294967295</v>
       </c>
     </row>
@@ -923,90 +1799,6 @@
       </c>
       <c r="P10" s="3" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15">
-        <v>8</v>
-      </c>
-      <c r="C15">
-        <v>16</v>
-      </c>
-      <c r="D15">
-        <v>32</v>
-      </c>
-      <c r="F15">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="4">
-        <f>-2^(B15-1)</f>
-        <v>-128</v>
-      </c>
-      <c r="C18" s="4">
-        <f>-2^(C15-1)</f>
-        <v>-32768</v>
-      </c>
-      <c r="D18" s="4">
-        <f>-2^(D15-1)</f>
-        <v>-2147483648</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="4">
-        <f>2 ^(B15-1) -1</f>
-        <v>127</v>
-      </c>
-      <c r="C19" s="4">
-        <f>2 ^(C15-1) -1</f>
-        <v>32767</v>
-      </c>
-      <c r="D19" s="4">
-        <f>2 ^(D15-1) -1</f>
-        <v>2147483647</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1015,30 +1807,6 @@
     <mergeCell ref="J1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add first jUnit 5 parameterized Test "i32_eqTest"  Add StringToIntegerConverter which converts decimal, hexadecimal, octal string to Integer.
</commit_message>
<xml_diff>
--- a/spec/Wasm Variable Types.xlsx
+++ b/spec/Wasm Variable Types.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="50">
   <si>
     <t>Min Value</t>
   </si>
@@ -414,13 +414,13 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -728,7 +728,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,7 +742,7 @@
     <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
     <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
@@ -866,6 +866,9 @@
       <c r="G4" s="12" t="s">
         <v>27</v>
       </c>
+      <c r="H4" s="11" t="s">
+        <v>16</v>
+      </c>
       <c r="I4" t="s">
         <v>40</v>
       </c>
@@ -892,6 +895,9 @@
       </c>
       <c r="G5" s="12" t="s">
         <v>36</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>16</v>
       </c>
       <c r="I5" t="s">
         <v>40</v>
@@ -1264,6 +1270,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="39.5703125" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
@@ -1290,10 +1297,10 @@
       <c r="C3" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="17"/>
+      <c r="E3" s="15"/>
       <c r="F3" t="s">
         <v>32</v>
       </c>
@@ -1308,10 +1315,10 @@
       <c r="C4">
         <v>16</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="15">
         <v>32</v>
       </c>
-      <c r="E4" s="17"/>
+      <c r="E4" s="15"/>
       <c r="F4">
         <v>64</v>
       </c>
@@ -1434,25 +1441,25 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">

</xml_diff>

<commit_message>
Update readme.md with latest progress.
</commit_message>
<xml_diff>
--- a/spec/Wasm Variable Types.xlsx
+++ b/spec/Wasm Variable Types.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="50">
   <si>
     <t>Min Value</t>
   </si>
@@ -414,13 +414,13 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -728,7 +728,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,7 +742,7 @@
     <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
@@ -866,9 +866,6 @@
       <c r="G4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>16</v>
-      </c>
       <c r="I4" t="s">
         <v>40</v>
       </c>
@@ -895,9 +892,6 @@
       </c>
       <c r="G5" s="12" t="s">
         <v>36</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>16</v>
       </c>
       <c r="I5" t="s">
         <v>40</v>
@@ -1270,7 +1264,6 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
@@ -1297,10 +1290,10 @@
       <c r="C3" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="15"/>
+      <c r="E3" s="17"/>
       <c r="F3" t="s">
         <v>32</v>
       </c>
@@ -1315,10 +1308,10 @@
       <c r="C4">
         <v>16</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="17">
         <v>32</v>
       </c>
-      <c r="E4" s="15"/>
+      <c r="E4" s="17"/>
       <c r="F4">
         <v>64</v>
       </c>
@@ -1441,25 +1434,25 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="17" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">

</xml_diff>